<commit_message>
Chose problems for Jan 27&28
</commit_message>
<xml_diff>
--- a/Reference/Problems_DB.xlsx
+++ b/Reference/Problems_DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\en908\Documents\GitHub\K_Coders_HKU\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20502E66-38CC-5B48-B3B7-3A843623ACB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FC118A-49AF-4DEB-9B08-F7738F52EA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{CCBF7CBE-323A-B946-A7A6-256A8E1F6F44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{CCBF7CBE-323A-B946-A7A6-256A8E1F6F44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="130">
   <si>
     <t>Number</t>
   </si>
@@ -322,17 +322,142 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/design-twitter/</t>
+  </si>
+  <si>
+    <t>HST001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorting</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/closest-numbers/problem?isFullScreen=true</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/closest-numbers/problem?isFullScreen=true</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closest Numbers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BST001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>좌표 압축</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/18870</t>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LST001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Sum</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/3sum/</t>
+  </si>
+  <si>
+    <t>LST002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Russian Doll Envelopes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/russian-doll-envelopes/</t>
+  </si>
+  <si>
+    <t>HST002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fradulent Activity Notifications</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hard</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BST002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>나이순 정렬</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/10814</t>
+  </si>
+  <si>
+    <t>https://www.acmicpc.net/problem/1181</t>
+  </si>
+  <si>
+    <t>BST003</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>단어 정렬</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HST003</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lily's Homework</t>
+  </si>
+  <si>
+    <t>https://www.hackerrank.com/challenges/lilys-homework/problem?isFullScreen=true</t>
+  </si>
+  <si>
+    <t>LST003</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-sorted-array/</t>
+  </si>
+  <si>
+    <t>Easy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Smallest Range Covering Elements from K Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/smallest-range-covering-elements-from-k-lists/</t>
+  </si>
+  <si>
+    <t>LST004</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -340,7 +465,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -348,8 +473,15 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -693,20 +825,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AEAD92-DF16-6F40-823D-6403D4A35067}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.3046875" customWidth="1"/>
+    <col min="3" max="3" width="25.3046875" customWidth="1"/>
     <col min="4" max="4" width="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -724,381 +856,381 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>83</v>
       </c>
@@ -1115,7 +1247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -1132,87 +1264,266 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>94</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C34" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E34" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+    <sortCondition ref="A38"/>
+  </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{D0D94381-7422-4B47-8C75-0A8E2CEA4AD8}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{35974DDB-64BD-F848-8DD7-DF3CB9E7DAA7}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{3958CBC5-586A-5541-A8BB-4BDDBC0C1F65}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{AE151E0D-C4C5-5546-AFC7-161EC7E9FAB2}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{61CB08F6-364E-FE49-A5D3-09122DA4227B}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{6B57C765-D45D-F44C-8616-1D6BD5421F23}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{8D1387EF-90DD-084D-98FE-314BF8F9F57C}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{A0CA9A4C-0BD3-A041-BD49-995C95759B08}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{609AB5D6-EB24-ED44-9443-D13384F26A8B}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{500CEA34-C770-F445-9D54-4DA9C0334044}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{F8B41769-1563-344D-A11D-630A0B1FEB18}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{A0306CCA-DE24-0243-98DE-7B6A52EA637A}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{AC05675A-E5D3-2746-B760-B9393E382D32}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{CD68637D-A11A-7A49-B56B-A402B8554DD4}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{455C8125-A033-F045-AD4D-24BAE43FDF84}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{1C164363-9938-BD4D-A10B-231B0ADE8AB6}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{545D8605-EEAB-624F-8FC7-38B9C19DCC0C}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{B102E35A-DCE5-214F-BE96-5406B6CC9F12}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{3758B887-C6ED-594A-8090-96771CF41F66}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{502DDED4-84AA-5743-A608-70DE50FA28B7}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{DA02D8FA-F5B0-FB4A-9F94-536BEA2D8768}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{2E4FE841-B68A-EA42-A797-29185F3B7936}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{D0D94381-7422-4B47-8C75-0A8E2CEA4AD8}"/>
+    <hyperlink ref="D26" r:id="rId2" xr:uid="{35974DDB-64BD-F848-8DD7-DF3CB9E7DAA7}"/>
+    <hyperlink ref="D14" r:id="rId3" xr:uid="{3958CBC5-586A-5541-A8BB-4BDDBC0C1F65}"/>
+    <hyperlink ref="D27" r:id="rId4" xr:uid="{AE151E0D-C4C5-5546-AFC7-161EC7E9FAB2}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{61CB08F6-364E-FE49-A5D3-09122DA4227B}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{6B57C765-D45D-F44C-8616-1D6BD5421F23}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{8D1387EF-90DD-084D-98FE-314BF8F9F57C}"/>
+    <hyperlink ref="D16" r:id="rId8" xr:uid="{A0CA9A4C-0BD3-A041-BD49-995C95759B08}"/>
+    <hyperlink ref="D28" r:id="rId9" xr:uid="{609AB5D6-EB24-ED44-9443-D13384F26A8B}"/>
+    <hyperlink ref="D29" r:id="rId10" xr:uid="{500CEA34-C770-F445-9D54-4DA9C0334044}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{F8B41769-1563-344D-A11D-630A0B1FEB18}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{A0306CCA-DE24-0243-98DE-7B6A52EA637A}"/>
+    <hyperlink ref="D30" r:id="rId13" xr:uid="{AC05675A-E5D3-2746-B760-B9393E382D32}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{CD68637D-A11A-7A49-B56B-A402B8554DD4}"/>
+    <hyperlink ref="D31" r:id="rId15" xr:uid="{455C8125-A033-F045-AD4D-24BAE43FDF84}"/>
+    <hyperlink ref="D8" r:id="rId16" xr:uid="{1C164363-9938-BD4D-A10B-231B0ADE8AB6}"/>
+    <hyperlink ref="D32" r:id="rId17" xr:uid="{545D8605-EEAB-624F-8FC7-38B9C19DCC0C}"/>
+    <hyperlink ref="D9" r:id="rId18" xr:uid="{B102E35A-DCE5-214F-BE96-5406B6CC9F12}"/>
+    <hyperlink ref="D10" r:id="rId19" xr:uid="{3758B887-C6ED-594A-8090-96771CF41F66}"/>
+    <hyperlink ref="D23" r:id="rId20" xr:uid="{502DDED4-84AA-5743-A608-70DE50FA28B7}"/>
+    <hyperlink ref="D11" r:id="rId21" xr:uid="{DA02D8FA-F5B0-FB4A-9F94-536BEA2D8768}"/>
+    <hyperlink ref="D12" r:id="rId22" xr:uid="{2E4FE841-B68A-EA42-A797-29185F3B7936}"/>
     <hyperlink ref="D24" r:id="rId23" xr:uid="{0EDCE016-B892-3740-BBE6-2DE947CFD5E6}"/>
     <hyperlink ref="D25" r:id="rId24" xr:uid="{7BDC6A29-D9CD-E049-9453-9F401184D2C9}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{EA8683FC-E326-9C43-9143-2E5897AE7C2E}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{903FF688-FD4B-384D-A059-E65B3BEA1867}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{43C88849-F2ED-B546-9D1F-E4B4591A9BFC}"/>
+    <hyperlink ref="D13" r:id="rId25" xr:uid="{EA8683FC-E326-9C43-9143-2E5897AE7C2E}"/>
+    <hyperlink ref="D33" r:id="rId26" xr:uid="{903FF688-FD4B-384D-A059-E65B3BEA1867}"/>
+    <hyperlink ref="D34" r:id="rId27" xr:uid="{43C88849-F2ED-B546-9D1F-E4B4591A9BFC}"/>
+    <hyperlink ref="D19" r:id="rId28" xr:uid="{6AD7A658-1E55-4418-9AB5-2E22DB0D9AA3}"/>
+    <hyperlink ref="D35" r:id="rId29" xr:uid="{3C2D14F9-1E64-445D-BA9E-B8340D10B822}"/>
+    <hyperlink ref="D20" r:id="rId30" xr:uid="{6E69E554-1145-4646-9583-AA1F699BE741}"/>
+    <hyperlink ref="D37" r:id="rId31" xr:uid="{22618222-381E-4910-A768-875C68720BF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>